<commit_message>
obs block jgr+cu examples
</commit_message>
<xml_diff>
--- a/results/cu_jgr/15x15/all/cu_jgr_all_15x15_True_2_0.2.xlsx
+++ b/results/cu_jgr/15x15/all/cu_jgr_all_15x15_True_2_0.2.xlsx
@@ -483,16 +483,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01479</v>
+        <v>0.00903</v>
       </c>
       <c r="E2" t="n">
-        <v>0.00739</v>
+        <v>0.00452</v>
       </c>
       <c r="F2" t="n">
-        <v>1.32183</v>
+        <v>0.8227100000000001</v>
       </c>
       <c r="G2" t="n">
         <v>0.85</v>
@@ -509,16 +509,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00717</v>
+        <v>0.006</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00358</v>
+        <v>0.003</v>
       </c>
       <c r="F3" t="n">
-        <v>0.76307</v>
+        <v>0.74091</v>
       </c>
       <c r="G3" t="n">
         <v>0.85</v>
@@ -535,16 +535,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>63</v>
+        <v>99</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00518</v>
+        <v>0.01006</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00259</v>
+        <v>0.00503</v>
       </c>
       <c r="F4" t="n">
-        <v>0.59211</v>
+        <v>1.2805</v>
       </c>
       <c r="G4" t="n">
         <v>0.85</v>
@@ -561,16 +561,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00759</v>
+        <v>0.00518</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0038</v>
+        <v>0.00259</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7749200000000001</v>
+        <v>0.74614</v>
       </c>
       <c r="G5" t="n">
         <v>0.85</v>
@@ -587,16 +587,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="D6" t="n">
-        <v>0.02137</v>
+        <v>0.02055</v>
       </c>
       <c r="E6" t="n">
-        <v>0.01068</v>
+        <v>0.01028</v>
       </c>
       <c r="F6" t="n">
-        <v>1.61688</v>
+        <v>1.8216</v>
       </c>
       <c r="G6" t="n">
         <v>0.85</v>
@@ -613,16 +613,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D7" t="n">
-        <v>0.01281</v>
+        <v>0.01507</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00641</v>
+        <v>0.00753</v>
       </c>
       <c r="F7" t="n">
-        <v>1.4041</v>
+        <v>1.73617</v>
       </c>
       <c r="G7" t="n">
         <v>0.85</v>
@@ -639,16 +639,16 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01698</v>
+        <v>0.0064</v>
       </c>
       <c r="E8" t="n">
-        <v>0.008489999999999999</v>
+        <v>0.0032</v>
       </c>
       <c r="F8" t="n">
-        <v>1.68522</v>
+        <v>0.9147999999999999</v>
       </c>
       <c r="G8" t="n">
         <v>0.85</v>
@@ -665,16 +665,16 @@
         <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0197</v>
+        <v>0.01495</v>
       </c>
       <c r="E9" t="n">
-        <v>0.009849999999999999</v>
+        <v>0.00748</v>
       </c>
       <c r="F9" t="n">
-        <v>2.47606</v>
+        <v>1.52111</v>
       </c>
       <c r="G9" t="n">
         <v>0.85</v>
@@ -691,16 +691,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02343</v>
+        <v>0.02426</v>
       </c>
       <c r="E10" t="n">
-        <v>0.01171</v>
+        <v>0.01213</v>
       </c>
       <c r="F10" t="n">
-        <v>1.92685</v>
+        <v>2.28353</v>
       </c>
       <c r="G10" t="n">
         <v>0.85</v>
@@ -717,16 +717,16 @@
         <v>1</v>
       </c>
       <c r="C11" t="n">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01421</v>
+        <v>0.01023</v>
       </c>
       <c r="E11" t="n">
-        <v>0.00711</v>
+        <v>0.00512</v>
       </c>
       <c r="F11" t="n">
-        <v>1.49125</v>
+        <v>0.94413</v>
       </c>
       <c r="G11" t="n">
         <v>0.85</v>
@@ -743,16 +743,16 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01415</v>
+        <v>0.01289</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00708</v>
+        <v>0.00644</v>
       </c>
       <c r="F12" t="n">
-        <v>1.63884</v>
+        <v>1.20449</v>
       </c>
       <c r="G12" t="n">
         <v>0.85</v>
@@ -769,16 +769,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0143</v>
+        <v>0.01027</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00715</v>
+        <v>0.00513</v>
       </c>
       <c r="F13" t="n">
-        <v>1.73013</v>
+        <v>1.15739</v>
       </c>
       <c r="G13" t="n">
         <v>0.85</v>
@@ -795,16 +795,16 @@
         <v>1</v>
       </c>
       <c r="C14" t="n">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="D14" t="n">
-        <v>0.00894</v>
+        <v>0.0132</v>
       </c>
       <c r="E14" t="n">
-        <v>0.00447</v>
+        <v>0.0066</v>
       </c>
       <c r="F14" t="n">
-        <v>1.44365</v>
+        <v>1.48963</v>
       </c>
       <c r="G14" t="n">
         <v>0.85</v>
@@ -821,16 +821,16 @@
         <v>1</v>
       </c>
       <c r="C15" t="n">
-        <v>148</v>
+        <v>107</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01027</v>
+        <v>0.008970000000000001</v>
       </c>
       <c r="E15" t="n">
-        <v>0.00513</v>
+        <v>0.00448</v>
       </c>
       <c r="F15" t="n">
-        <v>2.00402</v>
+        <v>1.4664</v>
       </c>
       <c r="G15" t="n">
         <v>0.85</v>
@@ -847,16 +847,16 @@
         <v>1</v>
       </c>
       <c r="C16" t="n">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="D16" t="n">
-        <v>0.02345</v>
+        <v>0.01645</v>
       </c>
       <c r="E16" t="n">
-        <v>0.01172</v>
+        <v>0.008229999999999999</v>
       </c>
       <c r="F16" t="n">
-        <v>2.83039</v>
+        <v>1.93468</v>
       </c>
       <c r="G16" t="n">
         <v>0.85</v>
@@ -873,16 +873,16 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>66</v>
+        <v>91</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01163</v>
+        <v>0.01566</v>
       </c>
       <c r="E17" t="n">
-        <v>0.00581</v>
+        <v>0.00783</v>
       </c>
       <c r="F17" t="n">
-        <v>1.0996</v>
+        <v>1.95395</v>
       </c>
       <c r="G17" t="n">
         <v>0.85</v>
@@ -899,16 +899,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01117</v>
+        <v>0.00812</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00558</v>
+        <v>0.00406</v>
       </c>
       <c r="F18" t="n">
-        <v>1.16088</v>
+        <v>1.06124</v>
       </c>
       <c r="G18" t="n">
         <v>0.85</v>
@@ -925,16 +925,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01036</v>
+        <v>0.01759</v>
       </c>
       <c r="E19" t="n">
-        <v>0.00518</v>
+        <v>0.008800000000000001</v>
       </c>
       <c r="F19" t="n">
-        <v>1.22132</v>
+        <v>1.96553</v>
       </c>
       <c r="G19" t="n">
         <v>0.85</v>
@@ -951,16 +951,16 @@
         <v>1</v>
       </c>
       <c r="C20" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01516</v>
+        <v>0.0117</v>
       </c>
       <c r="E20" t="n">
-        <v>0.00758</v>
+        <v>0.00585</v>
       </c>
       <c r="F20" t="n">
-        <v>1.28991</v>
+        <v>1.16631</v>
       </c>
       <c r="G20" t="n">
         <v>0.85</v>
@@ -977,16 +977,16 @@
         <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00876</v>
+        <v>0.01359</v>
       </c>
       <c r="E21" t="n">
-        <v>0.00438</v>
+        <v>0.0068</v>
       </c>
       <c r="F21" t="n">
-        <v>1.16859</v>
+        <v>1.43759</v>
       </c>
       <c r="G21" t="n">
         <v>0.85</v>
@@ -1003,16 +1003,16 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D22" t="n">
-        <v>0.02734</v>
+        <v>0.05546</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01367</v>
+        <v>0.02773</v>
       </c>
       <c r="F22" t="n">
-        <v>3.29524</v>
+        <v>3.47296</v>
       </c>
       <c r="G22" t="n">
         <v>0.15</v>
@@ -1029,16 +1029,16 @@
         <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0274</v>
+        <v>0.03864</v>
       </c>
       <c r="E23" t="n">
-        <v>0.0137</v>
+        <v>0.01932</v>
       </c>
       <c r="F23" t="n">
-        <v>1.73165</v>
+        <v>3.30533</v>
       </c>
       <c r="G23" t="n">
         <v>0.15</v>
@@ -1055,16 +1055,16 @@
         <v>1</v>
       </c>
       <c r="C24" t="n">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="D24" t="n">
-        <v>0.04992</v>
+        <v>0.03372</v>
       </c>
       <c r="E24" t="n">
-        <v>0.02496</v>
+        <v>0.01686</v>
       </c>
       <c r="F24" t="n">
-        <v>2.96455</v>
+        <v>3.12245</v>
       </c>
       <c r="G24" t="n">
         <v>0.15</v>
@@ -1081,16 +1081,16 @@
         <v>1</v>
       </c>
       <c r="C25" t="n">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D25" t="n">
-        <v>0.03388</v>
+        <v>0.04921</v>
       </c>
       <c r="E25" t="n">
-        <v>0.01694</v>
+        <v>0.0246</v>
       </c>
       <c r="F25" t="n">
-        <v>2.68301</v>
+        <v>3.09036</v>
       </c>
       <c r="G25" t="n">
         <v>0.15</v>
@@ -1107,16 +1107,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="D26" t="n">
-        <v>0.03858</v>
+        <v>0.0299</v>
       </c>
       <c r="E26" t="n">
-        <v>0.01929</v>
+        <v>0.01495</v>
       </c>
       <c r="F26" t="n">
-        <v>2.74795</v>
+        <v>2.97875</v>
       </c>
       <c r="G26" t="n">
         <v>0.15</v>
@@ -1133,16 +1133,16 @@
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="D27" t="n">
-        <v>0.03524</v>
+        <v>0.05758</v>
       </c>
       <c r="E27" t="n">
-        <v>0.01762</v>
+        <v>0.02879</v>
       </c>
       <c r="F27" t="n">
-        <v>2.95832</v>
+        <v>5.78714</v>
       </c>
       <c r="G27" t="n">
         <v>0.15</v>
@@ -1159,16 +1159,16 @@
         <v>1</v>
       </c>
       <c r="C28" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0495</v>
+        <v>0.04379</v>
       </c>
       <c r="E28" t="n">
-        <v>0.02475</v>
+        <v>0.02189</v>
       </c>
       <c r="F28" t="n">
-        <v>2.74199</v>
+        <v>3.06089</v>
       </c>
       <c r="G28" t="n">
         <v>0.15</v>
@@ -1185,16 +1185,16 @@
         <v>1</v>
       </c>
       <c r="C29" t="n">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D29" t="n">
-        <v>0.03501</v>
+        <v>0.04567</v>
       </c>
       <c r="E29" t="n">
-        <v>0.01751</v>
+        <v>0.02283</v>
       </c>
       <c r="F29" t="n">
-        <v>3.04041</v>
+        <v>3.6214</v>
       </c>
       <c r="G29" t="n">
         <v>0.15</v>
@@ -1211,16 +1211,16 @@
         <v>1</v>
       </c>
       <c r="C30" t="n">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="D30" t="n">
-        <v>0.02264</v>
+        <v>0.03232</v>
       </c>
       <c r="E30" t="n">
-        <v>0.01132</v>
+        <v>0.01616</v>
       </c>
       <c r="F30" t="n">
-        <v>2.08905</v>
+        <v>3.58289</v>
       </c>
       <c r="G30" t="n">
         <v>0.15</v>
@@ -1237,16 +1237,16 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D31" t="n">
-        <v>0.04048</v>
+        <v>0.04084</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02024</v>
+        <v>0.02042</v>
       </c>
       <c r="F31" t="n">
-        <v>2.50762</v>
+        <v>3.26442</v>
       </c>
       <c r="G31" t="n">
         <v>0.15</v>
@@ -1263,16 +1263,16 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D32" t="n">
-        <v>0.03934</v>
+        <v>0.05118</v>
       </c>
       <c r="E32" t="n">
-        <v>0.01967</v>
+        <v>0.02559</v>
       </c>
       <c r="F32" t="n">
-        <v>3.46194</v>
+        <v>2.71006</v>
       </c>
       <c r="G32" t="n">
         <v>0.15</v>
@@ -1289,16 +1289,16 @@
         <v>1</v>
       </c>
       <c r="C33" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D33" t="n">
-        <v>0.01973</v>
+        <v>0.04718</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00987</v>
+        <v>0.02359</v>
       </c>
       <c r="F33" t="n">
-        <v>1.75995</v>
+        <v>3.78283</v>
       </c>
       <c r="G33" t="n">
         <v>0.15</v>
@@ -1315,16 +1315,16 @@
         <v>1</v>
       </c>
       <c r="C34" t="n">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="D34" t="n">
-        <v>0.01766</v>
+        <v>0.04309</v>
       </c>
       <c r="E34" t="n">
-        <v>0.008829999999999999</v>
+        <v>0.02155</v>
       </c>
       <c r="F34" t="n">
-        <v>1.56839</v>
+        <v>2.54969</v>
       </c>
       <c r="G34" t="n">
         <v>0.15</v>
@@ -1341,16 +1341,16 @@
         <v>1</v>
       </c>
       <c r="C35" t="n">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02951</v>
+        <v>0.03394</v>
       </c>
       <c r="E35" t="n">
-        <v>0.01476</v>
+        <v>0.01697</v>
       </c>
       <c r="F35" t="n">
-        <v>2.13749</v>
+        <v>2.71734</v>
       </c>
       <c r="G35" t="n">
         <v>0.15</v>
@@ -1367,16 +1367,16 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D36" t="n">
-        <v>0.03657</v>
+        <v>0.05379</v>
       </c>
       <c r="E36" t="n">
-        <v>0.01828</v>
+        <v>0.02689</v>
       </c>
       <c r="F36" t="n">
-        <v>2.86445</v>
+        <v>3.64792</v>
       </c>
       <c r="G36" t="n">
         <v>0.15</v>
@@ -1393,16 +1393,16 @@
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="D37" t="n">
-        <v>0.04337</v>
+        <v>0.03739</v>
       </c>
       <c r="E37" t="n">
-        <v>0.02168</v>
+        <v>0.01869</v>
       </c>
       <c r="F37" t="n">
-        <v>3.62282</v>
+        <v>2.30812</v>
       </c>
       <c r="G37" t="n">
         <v>0.15</v>
@@ -1419,16 +1419,16 @@
         <v>1</v>
       </c>
       <c r="C38" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D38" t="n">
-        <v>0.02681</v>
+        <v>0.03219</v>
       </c>
       <c r="E38" t="n">
-        <v>0.0134</v>
+        <v>0.01609</v>
       </c>
       <c r="F38" t="n">
-        <v>1.88857</v>
+        <v>2.30328</v>
       </c>
       <c r="G38" t="n">
         <v>0.15</v>
@@ -1445,16 +1445,16 @@
         <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="D39" t="n">
-        <v>0.02409</v>
+        <v>0.04842</v>
       </c>
       <c r="E39" t="n">
-        <v>0.01204</v>
+        <v>0.02421</v>
       </c>
       <c r="F39" t="n">
-        <v>1.74362</v>
+        <v>3.94917</v>
       </c>
       <c r="G39" t="n">
         <v>0.15</v>
@@ -1471,16 +1471,16 @@
         <v>1</v>
       </c>
       <c r="C40" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D40" t="n">
-        <v>0.02292</v>
+        <v>0.05139</v>
       </c>
       <c r="E40" t="n">
-        <v>0.01146</v>
+        <v>0.0257</v>
       </c>
       <c r="F40" t="n">
-        <v>2.10733</v>
+        <v>4.33623</v>
       </c>
       <c r="G40" t="n">
         <v>0.15</v>
@@ -1497,16 +1497,16 @@
         <v>1</v>
       </c>
       <c r="C41" t="n">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0413</v>
+        <v>0.0495</v>
       </c>
       <c r="E41" t="n">
-        <v>0.02065</v>
+        <v>0.02475</v>
       </c>
       <c r="F41" t="n">
-        <v>3.4116</v>
+        <v>4.29095</v>
       </c>
       <c r="G41" t="n">
         <v>0.15</v>
@@ -1523,16 +1523,16 @@
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D42" t="n">
-        <v>0.06178</v>
+        <v>0.06475</v>
       </c>
       <c r="E42" t="n">
-        <v>0.01545</v>
+        <v>0.01619</v>
       </c>
       <c r="F42" t="n">
-        <v>4.29858</v>
+        <v>2.55932</v>
       </c>
       <c r="G42" t="n">
         <v>0.15</v>
@@ -1549,16 +1549,16 @@
         <v>1</v>
       </c>
       <c r="C43" t="n">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D43" t="n">
-        <v>0.04504</v>
+        <v>0.07575999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>0.01126</v>
+        <v>0.01894</v>
       </c>
       <c r="F43" t="n">
-        <v>2.90405</v>
+        <v>5.03086</v>
       </c>
       <c r="G43" t="n">
         <v>0.15</v>
@@ -1575,16 +1575,16 @@
         <v>1</v>
       </c>
       <c r="C44" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D44" t="n">
-        <v>0.02487</v>
+        <v>0.03952</v>
       </c>
       <c r="E44" t="n">
-        <v>0.00622</v>
+        <v>0.00988</v>
       </c>
       <c r="F44" t="n">
-        <v>1.46847</v>
+        <v>2.52926</v>
       </c>
       <c r="G44" t="n">
         <v>0.15</v>
@@ -1601,16 +1601,16 @@
         <v>1</v>
       </c>
       <c r="C45" t="n">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D45" t="n">
-        <v>0.06543</v>
+        <v>0.09866</v>
       </c>
       <c r="E45" t="n">
-        <v>0.01636</v>
+        <v>0.02466</v>
       </c>
       <c r="F45" t="n">
-        <v>3.02128</v>
+        <v>5.49727</v>
       </c>
       <c r="G45" t="n">
         <v>0.15</v>
@@ -1627,16 +1627,16 @@
         <v>1</v>
       </c>
       <c r="C46" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D46" t="n">
-        <v>0.08099000000000001</v>
+        <v>0.05678</v>
       </c>
       <c r="E46" t="n">
-        <v>0.02025</v>
+        <v>0.0142</v>
       </c>
       <c r="F46" t="n">
-        <v>3.56079</v>
+        <v>3.1014</v>
       </c>
       <c r="G46" t="n">
         <v>0.15</v>
@@ -1653,16 +1653,16 @@
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D47" t="n">
-        <v>0.02886</v>
+        <v>0.06269</v>
       </c>
       <c r="E47" t="n">
-        <v>0.00722</v>
+        <v>0.01567</v>
       </c>
       <c r="F47" t="n">
-        <v>1.97472</v>
+        <v>3.88929</v>
       </c>
       <c r="G47" t="n">
         <v>0.15</v>
@@ -1679,16 +1679,16 @@
         <v>1</v>
       </c>
       <c r="C48" t="n">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0242</v>
+        <v>0.0742</v>
       </c>
       <c r="E48" t="n">
-        <v>0.00605</v>
+        <v>0.01855</v>
       </c>
       <c r="F48" t="n">
-        <v>1.77931</v>
+        <v>2.73403</v>
       </c>
       <c r="G48" t="n">
         <v>0.15</v>
@@ -1705,16 +1705,16 @@
         <v>1</v>
       </c>
       <c r="C49" t="n">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D49" t="n">
-        <v>0.04032</v>
+        <v>0.05722</v>
       </c>
       <c r="E49" t="n">
-        <v>0.01008</v>
+        <v>0.01431</v>
       </c>
       <c r="F49" t="n">
-        <v>2.29961</v>
+        <v>2.80463</v>
       </c>
       <c r="G49" t="n">
         <v>0.15</v>
@@ -1731,16 +1731,16 @@
         <v>1</v>
       </c>
       <c r="C50" t="n">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D50" t="n">
-        <v>0.06048</v>
+        <v>0.06101</v>
       </c>
       <c r="E50" t="n">
-        <v>0.01512</v>
+        <v>0.01525</v>
       </c>
       <c r="F50" t="n">
-        <v>4.04938</v>
+        <v>4.65033</v>
       </c>
       <c r="G50" t="n">
         <v>0.15</v>
@@ -1757,16 +1757,16 @@
         <v>1</v>
       </c>
       <c r="C51" t="n">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="D51" t="n">
-        <v>0.05122</v>
+        <v>0.08211</v>
       </c>
       <c r="E51" t="n">
-        <v>0.01281</v>
+        <v>0.02053</v>
       </c>
       <c r="F51" t="n">
-        <v>2.72042</v>
+        <v>6.05909</v>
       </c>
       <c r="G51" t="n">
         <v>0.15</v>
@@ -1783,16 +1783,16 @@
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="D52" t="n">
-        <v>0.06856</v>
+        <v>0.05591</v>
       </c>
       <c r="E52" t="n">
-        <v>0.01714</v>
+        <v>0.01398</v>
       </c>
       <c r="F52" t="n">
-        <v>2.91086</v>
+        <v>3.96914</v>
       </c>
       <c r="G52" t="n">
         <v>0.15</v>
@@ -1809,16 +1809,16 @@
         <v>1</v>
       </c>
       <c r="C53" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D53" t="n">
-        <v>0.03645</v>
+        <v>0.05817</v>
       </c>
       <c r="E53" t="n">
-        <v>0.00911</v>
+        <v>0.01454</v>
       </c>
       <c r="F53" t="n">
-        <v>2.47277</v>
+        <v>3.08853</v>
       </c>
       <c r="G53" t="n">
         <v>0.15</v>
@@ -1835,16 +1835,16 @@
         <v>1</v>
       </c>
       <c r="C54" t="n">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="D54" t="n">
-        <v>0.03551</v>
+        <v>0.09257</v>
       </c>
       <c r="E54" t="n">
-        <v>0.008880000000000001</v>
+        <v>0.02314</v>
       </c>
       <c r="F54" t="n">
-        <v>2.76496</v>
+        <v>4.60969</v>
       </c>
       <c r="G54" t="n">
         <v>0.15</v>
@@ -1861,16 +1861,16 @@
         <v>1</v>
       </c>
       <c r="C55" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D55" t="n">
-        <v>0.02588</v>
+        <v>0.06308999999999999</v>
       </c>
       <c r="E55" t="n">
-        <v>0.00647</v>
+        <v>0.01577</v>
       </c>
       <c r="F55" t="n">
-        <v>1.77427</v>
+        <v>2.94291</v>
       </c>
       <c r="G55" t="n">
         <v>0.15</v>
@@ -1887,16 +1887,16 @@
         <v>1</v>
       </c>
       <c r="C56" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D56" t="n">
-        <v>0.05185</v>
+        <v>0.04208</v>
       </c>
       <c r="E56" t="n">
-        <v>0.01296</v>
+        <v>0.01052</v>
       </c>
       <c r="F56" t="n">
-        <v>2.90531</v>
+        <v>2.52365</v>
       </c>
       <c r="G56" t="n">
         <v>0.15</v>
@@ -1913,16 +1913,16 @@
         <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D57" t="n">
-        <v>0.07048</v>
+        <v>0.05897</v>
       </c>
       <c r="E57" t="n">
-        <v>0.01762</v>
+        <v>0.01474</v>
       </c>
       <c r="F57" t="n">
-        <v>3.89703</v>
+        <v>3.74415</v>
       </c>
       <c r="G57" t="n">
         <v>0.15</v>
@@ -1939,16 +1939,16 @@
         <v>1</v>
       </c>
       <c r="C58" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D58" t="n">
-        <v>0.02618</v>
+        <v>0.05181</v>
       </c>
       <c r="E58" t="n">
-        <v>0.00654</v>
+        <v>0.01295</v>
       </c>
       <c r="F58" t="n">
-        <v>1.93439</v>
+        <v>3.6249</v>
       </c>
       <c r="G58" t="n">
         <v>0.15</v>
@@ -1965,16 +1965,16 @@
         <v>1</v>
       </c>
       <c r="C59" t="n">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D59" t="n">
-        <v>0.0248</v>
+        <v>0.05697</v>
       </c>
       <c r="E59" t="n">
-        <v>0.0062</v>
+        <v>0.01424</v>
       </c>
       <c r="F59" t="n">
-        <v>1.52674</v>
+        <v>3.64648</v>
       </c>
       <c r="G59" t="n">
         <v>0.15</v>
@@ -1991,16 +1991,16 @@
         <v>1</v>
       </c>
       <c r="C60" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D60" t="n">
-        <v>0.04914</v>
+        <v>0.05363</v>
       </c>
       <c r="E60" t="n">
-        <v>0.01229</v>
+        <v>0.01341</v>
       </c>
       <c r="F60" t="n">
-        <v>2.75817</v>
+        <v>2.60343</v>
       </c>
       <c r="G60" t="n">
         <v>0.15</v>
@@ -2017,16 +2017,16 @@
         <v>1</v>
       </c>
       <c r="C61" t="n">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D61" t="n">
-        <v>0.03145</v>
+        <v>0.03798</v>
       </c>
       <c r="E61" t="n">
-        <v>0.007860000000000001</v>
+        <v>0.00949</v>
       </c>
       <c r="F61" t="n">
-        <v>1.72979</v>
+        <v>1.768</v>
       </c>
       <c r="G61" t="n">
         <v>0.15</v>
@@ -2043,16 +2043,16 @@
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D62" t="n">
-        <v>0.03765</v>
+        <v>0.02415</v>
       </c>
       <c r="E62" t="n">
-        <v>0.00941</v>
+        <v>0.00604</v>
       </c>
       <c r="F62" t="n">
-        <v>2.16843</v>
+        <v>2.11833</v>
       </c>
       <c r="G62" t="n">
         <v>0.85</v>
@@ -2069,16 +2069,16 @@
         <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D63" t="n">
-        <v>0.0149</v>
+        <v>0.02525</v>
       </c>
       <c r="E63" t="n">
-        <v>0.00372</v>
+        <v>0.00631</v>
       </c>
       <c r="F63" t="n">
-        <v>1.20473</v>
+        <v>2.39355</v>
       </c>
       <c r="G63" t="n">
         <v>0.85</v>
@@ -2095,16 +2095,16 @@
         <v>1</v>
       </c>
       <c r="C64" t="n">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="D64" t="n">
-        <v>0.01933</v>
+        <v>0.02155</v>
       </c>
       <c r="E64" t="n">
-        <v>0.00483</v>
+        <v>0.00539</v>
       </c>
       <c r="F64" t="n">
-        <v>1.93431</v>
+        <v>1.76452</v>
       </c>
       <c r="G64" t="n">
         <v>0.85</v>
@@ -2121,16 +2121,16 @@
         <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D65" t="n">
-        <v>0.02233</v>
+        <v>0.03395</v>
       </c>
       <c r="E65" t="n">
-        <v>0.00558</v>
+        <v>0.008489999999999999</v>
       </c>
       <c r="F65" t="n">
-        <v>1.46421</v>
+        <v>2.48558</v>
       </c>
       <c r="G65" t="n">
         <v>0.85</v>
@@ -2147,16 +2147,16 @@
         <v>1</v>
       </c>
       <c r="C66" t="n">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D66" t="n">
-        <v>0.01136</v>
+        <v>0.03931</v>
       </c>
       <c r="E66" t="n">
-        <v>0.00284</v>
+        <v>0.00983</v>
       </c>
       <c r="F66" t="n">
-        <v>1.06481</v>
+        <v>2.41871</v>
       </c>
       <c r="G66" t="n">
         <v>0.85</v>
@@ -2173,16 +2173,16 @@
         <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D67" t="n">
-        <v>0.01749</v>
+        <v>0.02739</v>
       </c>
       <c r="E67" t="n">
-        <v>0.00437</v>
+        <v>0.00685</v>
       </c>
       <c r="F67" t="n">
-        <v>1.29164</v>
+        <v>2.30805</v>
       </c>
       <c r="G67" t="n">
         <v>0.85</v>
@@ -2199,16 +2199,16 @@
         <v>1</v>
       </c>
       <c r="C68" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D68" t="n">
-        <v>0.03039</v>
+        <v>0.05116</v>
       </c>
       <c r="E68" t="n">
-        <v>0.0076</v>
+        <v>0.01279</v>
       </c>
       <c r="F68" t="n">
-        <v>1.35733</v>
+        <v>2.4429</v>
       </c>
       <c r="G68" t="n">
         <v>0.85</v>
@@ -2225,16 +2225,16 @@
         <v>1</v>
       </c>
       <c r="C69" t="n">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D69" t="n">
-        <v>0.01266</v>
+        <v>0.04814</v>
       </c>
       <c r="E69" t="n">
-        <v>0.00317</v>
+        <v>0.01203</v>
       </c>
       <c r="F69" t="n">
-        <v>1.60433</v>
+        <v>2.77841</v>
       </c>
       <c r="G69" t="n">
         <v>0.85</v>
@@ -2251,16 +2251,16 @@
         <v>1</v>
       </c>
       <c r="C70" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D70" t="n">
-        <v>0.02</v>
+        <v>0.03537</v>
       </c>
       <c r="E70" t="n">
-        <v>0.005</v>
+        <v>0.008840000000000001</v>
       </c>
       <c r="F70" t="n">
-        <v>1.41256</v>
+        <v>2.41606</v>
       </c>
       <c r="G70" t="n">
         <v>0.85</v>
@@ -2277,16 +2277,16 @@
         <v>1</v>
       </c>
       <c r="C71" t="n">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D71" t="n">
-        <v>0.02668</v>
+        <v>0.04138</v>
       </c>
       <c r="E71" t="n">
-        <v>0.00667</v>
+        <v>0.01035</v>
       </c>
       <c r="F71" t="n">
-        <v>1.70293</v>
+        <v>2.36213</v>
       </c>
       <c r="G71" t="n">
         <v>0.85</v>
@@ -2303,16 +2303,16 @@
         <v>1</v>
       </c>
       <c r="C72" t="n">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D72" t="n">
-        <v>0.02408</v>
+        <v>0.04331</v>
       </c>
       <c r="E72" t="n">
-        <v>0.00602</v>
+        <v>0.01083</v>
       </c>
       <c r="F72" t="n">
-        <v>2.26134</v>
+        <v>2.20987</v>
       </c>
       <c r="G72" t="n">
         <v>0.85</v>
@@ -2329,16 +2329,16 @@
         <v>1</v>
       </c>
       <c r="C73" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D73" t="n">
-        <v>0.03299</v>
+        <v>0.01782</v>
       </c>
       <c r="E73" t="n">
-        <v>0.00825</v>
+        <v>0.00445</v>
       </c>
       <c r="F73" t="n">
-        <v>2.44952</v>
+        <v>1.36332</v>
       </c>
       <c r="G73" t="n">
         <v>0.85</v>
@@ -2355,16 +2355,16 @@
         <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D74" t="n">
-        <v>0.01581</v>
+        <v>0.01163</v>
       </c>
       <c r="E74" t="n">
-        <v>0.00395</v>
+        <v>0.00291</v>
       </c>
       <c r="F74" t="n">
-        <v>1.40423</v>
+        <v>1.07828</v>
       </c>
       <c r="G74" t="n">
         <v>0.85</v>
@@ -2381,16 +2381,16 @@
         <v>1</v>
       </c>
       <c r="C75" t="n">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D75" t="n">
-        <v>0.01641</v>
+        <v>0.01605</v>
       </c>
       <c r="E75" t="n">
-        <v>0.0041</v>
+        <v>0.00401</v>
       </c>
       <c r="F75" t="n">
-        <v>1.08455</v>
+        <v>1.23361</v>
       </c>
       <c r="G75" t="n">
         <v>0.85</v>
@@ -2407,16 +2407,16 @@
         <v>1</v>
       </c>
       <c r="C76" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D76" t="n">
-        <v>0.01603</v>
+        <v>0.0192</v>
       </c>
       <c r="E76" t="n">
-        <v>0.00401</v>
+        <v>0.0048</v>
       </c>
       <c r="F76" t="n">
-        <v>1.28351</v>
+        <v>1.25834</v>
       </c>
       <c r="G76" t="n">
         <v>0.85</v>
@@ -2433,16 +2433,16 @@
         <v>1</v>
       </c>
       <c r="C77" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D77" t="n">
-        <v>0.01655</v>
+        <v>0.02107</v>
       </c>
       <c r="E77" t="n">
-        <v>0.00414</v>
+        <v>0.00527</v>
       </c>
       <c r="F77" t="n">
-        <v>1.08231</v>
+        <v>1.16733</v>
       </c>
       <c r="G77" t="n">
         <v>0.85</v>
@@ -2459,16 +2459,16 @@
         <v>1</v>
       </c>
       <c r="C78" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D78" t="n">
-        <v>0.01859</v>
+        <v>0.01387</v>
       </c>
       <c r="E78" t="n">
-        <v>0.00465</v>
+        <v>0.00347</v>
       </c>
       <c r="F78" t="n">
-        <v>1.24891</v>
+        <v>1.01501</v>
       </c>
       <c r="G78" t="n">
         <v>0.85</v>
@@ -2485,16 +2485,16 @@
         <v>1</v>
       </c>
       <c r="C79" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D79" t="n">
-        <v>0.02812</v>
+        <v>0.012</v>
       </c>
       <c r="E79" t="n">
-        <v>0.00703</v>
+        <v>0.003</v>
       </c>
       <c r="F79" t="n">
-        <v>1.41618</v>
+        <v>0.88563</v>
       </c>
       <c r="G79" t="n">
         <v>0.85</v>
@@ -2511,16 +2511,16 @@
         <v>1</v>
       </c>
       <c r="C80" t="n">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="D80" t="n">
-        <v>0.02138</v>
+        <v>0.01782</v>
       </c>
       <c r="E80" t="n">
-        <v>0.00535</v>
+        <v>0.00446</v>
       </c>
       <c r="F80" t="n">
-        <v>1.59929</v>
+        <v>1.93906</v>
       </c>
       <c r="G80" t="n">
         <v>0.85</v>
@@ -2537,16 +2537,16 @@
         <v>1</v>
       </c>
       <c r="C81" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D81" t="n">
-        <v>0.02072</v>
+        <v>0.02285</v>
       </c>
       <c r="E81" t="n">
-        <v>0.00518</v>
+        <v>0.00571</v>
       </c>
       <c r="F81" t="n">
-        <v>0.99973</v>
+        <v>1.08401</v>
       </c>
       <c r="G81" t="n">
         <v>0.85</v>
@@ -2563,16 +2563,16 @@
         <v>1</v>
       </c>
       <c r="C82" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D82" t="n">
-        <v>0.04275</v>
+        <v>0.04869</v>
       </c>
       <c r="E82" t="n">
-        <v>0.00713</v>
+        <v>0.008109999999999999</v>
       </c>
       <c r="F82" t="n">
-        <v>1.84804</v>
+        <v>1.93713</v>
       </c>
       <c r="G82" t="n">
         <v>0.85</v>
@@ -2589,16 +2589,16 @@
         <v>1</v>
       </c>
       <c r="C83" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D83" t="n">
-        <v>0.05703</v>
+        <v>0.05738</v>
       </c>
       <c r="E83" t="n">
-        <v>0.0095</v>
+        <v>0.009560000000000001</v>
       </c>
       <c r="F83" t="n">
-        <v>1.8046</v>
+        <v>2.46424</v>
       </c>
       <c r="G83" t="n">
         <v>0.85</v>
@@ -2615,16 +2615,16 @@
         <v>1</v>
       </c>
       <c r="C84" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D84" t="n">
-        <v>0.0327</v>
+        <v>0.02138</v>
       </c>
       <c r="E84" t="n">
-        <v>0.00545</v>
+        <v>0.00356</v>
       </c>
       <c r="F84" t="n">
-        <v>1.59965</v>
+        <v>1.15466</v>
       </c>
       <c r="G84" t="n">
         <v>0.85</v>
@@ -2641,16 +2641,16 @@
         <v>1</v>
       </c>
       <c r="C85" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D85" t="n">
-        <v>0.04494</v>
+        <v>0.02823</v>
       </c>
       <c r="E85" t="n">
-        <v>0.00749</v>
+        <v>0.00471</v>
       </c>
       <c r="F85" t="n">
-        <v>2.17787</v>
+        <v>1.18467</v>
       </c>
       <c r="G85" t="n">
         <v>0.85</v>
@@ -2667,16 +2667,16 @@
         <v>1</v>
       </c>
       <c r="C86" t="n">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D86" t="n">
-        <v>0.02011</v>
+        <v>0.02566</v>
       </c>
       <c r="E86" t="n">
-        <v>0.00335</v>
+        <v>0.00428</v>
       </c>
       <c r="F86" t="n">
-        <v>1.05661</v>
+        <v>1.10434</v>
       </c>
       <c r="G86" t="n">
         <v>0.85</v>
@@ -2693,16 +2693,16 @@
         <v>1</v>
       </c>
       <c r="C87" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D87" t="n">
-        <v>0.0247</v>
+        <v>0.032</v>
       </c>
       <c r="E87" t="n">
-        <v>0.00412</v>
+        <v>0.00533</v>
       </c>
       <c r="F87" t="n">
-        <v>1.25783</v>
+        <v>1.32742</v>
       </c>
       <c r="G87" t="n">
         <v>0.85</v>
@@ -2719,16 +2719,16 @@
         <v>1</v>
       </c>
       <c r="C88" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D88" t="n">
-        <v>0.02181</v>
+        <v>0.02269</v>
       </c>
       <c r="E88" t="n">
-        <v>0.00363</v>
+        <v>0.00378</v>
       </c>
       <c r="F88" t="n">
-        <v>1.17459</v>
+        <v>1.2618</v>
       </c>
       <c r="G88" t="n">
         <v>0.85</v>
@@ -2745,16 +2745,16 @@
         <v>1</v>
       </c>
       <c r="C89" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D89" t="n">
-        <v>0.04382</v>
+        <v>0.01359</v>
       </c>
       <c r="E89" t="n">
-        <v>0.0073</v>
+        <v>0.00227</v>
       </c>
       <c r="F89" t="n">
-        <v>2.34955</v>
+        <v>0.78191</v>
       </c>
       <c r="G89" t="n">
         <v>0.85</v>
@@ -2771,16 +2771,16 @@
         <v>1</v>
       </c>
       <c r="C90" t="n">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D90" t="n">
-        <v>0.01924</v>
+        <v>0.02628</v>
       </c>
       <c r="E90" t="n">
-        <v>0.00321</v>
+        <v>0.00438</v>
       </c>
       <c r="F90" t="n">
-        <v>1.43788</v>
+        <v>1.33309</v>
       </c>
       <c r="G90" t="n">
         <v>0.85</v>
@@ -2797,16 +2797,16 @@
         <v>1</v>
       </c>
       <c r="C91" t="n">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="D91" t="n">
-        <v>0.03864</v>
+        <v>0.03281</v>
       </c>
       <c r="E91" t="n">
-        <v>0.00644</v>
+        <v>0.00547</v>
       </c>
       <c r="F91" t="n">
-        <v>1.35757</v>
+        <v>1.59595</v>
       </c>
       <c r="G91" t="n">
         <v>0.85</v>
@@ -2826,13 +2826,13 @@
         <v>22</v>
       </c>
       <c r="D92" t="n">
-        <v>0.04235</v>
+        <v>0.01423</v>
       </c>
       <c r="E92" t="n">
-        <v>0.00706</v>
+        <v>0.00237</v>
       </c>
       <c r="F92" t="n">
-        <v>1.95604</v>
+        <v>0.9828</v>
       </c>
       <c r="G92" t="n">
         <v>0.85</v>
@@ -2849,16 +2849,16 @@
         <v>1</v>
       </c>
       <c r="C93" t="n">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D93" t="n">
-        <v>0.0372</v>
+        <v>0.01933</v>
       </c>
       <c r="E93" t="n">
-        <v>0.0062</v>
+        <v>0.00322</v>
       </c>
       <c r="F93" t="n">
-        <v>2.19313</v>
+        <v>1.70926</v>
       </c>
       <c r="G93" t="n">
         <v>0.85</v>
@@ -2875,16 +2875,16 @@
         <v>1</v>
       </c>
       <c r="C94" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D94" t="n">
-        <v>0.02258</v>
+        <v>0.03287</v>
       </c>
       <c r="E94" t="n">
-        <v>0.00376</v>
+        <v>0.00548</v>
       </c>
       <c r="F94" t="n">
-        <v>1.10031</v>
+        <v>1.48617</v>
       </c>
       <c r="G94" t="n">
         <v>0.85</v>
@@ -2901,16 +2901,16 @@
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D95" t="n">
-        <v>0.04987</v>
+        <v>0.02981</v>
       </c>
       <c r="E95" t="n">
-        <v>0.00831</v>
+        <v>0.00497</v>
       </c>
       <c r="F95" t="n">
-        <v>2.15277</v>
+        <v>1.50514</v>
       </c>
       <c r="G95" t="n">
         <v>0.85</v>
@@ -2927,16 +2927,16 @@
         <v>1</v>
       </c>
       <c r="C96" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D96" t="n">
-        <v>0.04087</v>
+        <v>0.04847</v>
       </c>
       <c r="E96" t="n">
-        <v>0.00681</v>
+        <v>0.00808</v>
       </c>
       <c r="F96" t="n">
-        <v>2.66495</v>
+        <v>2.5096</v>
       </c>
       <c r="G96" t="n">
         <v>0.85</v>
@@ -2953,16 +2953,16 @@
         <v>1</v>
       </c>
       <c r="C97" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D97" t="n">
-        <v>0.03343</v>
+        <v>0.06598</v>
       </c>
       <c r="E97" t="n">
-        <v>0.00557</v>
+        <v>0.011</v>
       </c>
       <c r="F97" t="n">
-        <v>1.21354</v>
+        <v>2.47177</v>
       </c>
       <c r="G97" t="n">
         <v>0.85</v>
@@ -2982,13 +2982,13 @@
         <v>22</v>
       </c>
       <c r="D98" t="n">
-        <v>0.02841</v>
+        <v>0.06016</v>
       </c>
       <c r="E98" t="n">
-        <v>0.00473</v>
+        <v>0.01003</v>
       </c>
       <c r="F98" t="n">
-        <v>1.35838</v>
+        <v>2.48518</v>
       </c>
       <c r="G98" t="n">
         <v>0.85</v>
@@ -3005,16 +3005,16 @@
         <v>1</v>
       </c>
       <c r="C99" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D99" t="n">
-        <v>0.02381</v>
+        <v>0.03985</v>
       </c>
       <c r="E99" t="n">
-        <v>0.00397</v>
+        <v>0.00664</v>
       </c>
       <c r="F99" t="n">
-        <v>1.20449</v>
+        <v>2.2877</v>
       </c>
       <c r="G99" t="n">
         <v>0.85</v>
@@ -3031,16 +3031,16 @@
         <v>1</v>
       </c>
       <c r="C100" t="n">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D100" t="n">
-        <v>0.02638</v>
+        <v>0.06099</v>
       </c>
       <c r="E100" t="n">
-        <v>0.0044</v>
+        <v>0.01017</v>
       </c>
       <c r="F100" t="n">
-        <v>1.38594</v>
+        <v>2.11035</v>
       </c>
       <c r="G100" t="n">
         <v>0.85</v>
@@ -3057,16 +3057,16 @@
         <v>1</v>
       </c>
       <c r="C101" t="n">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D101" t="n">
-        <v>0.02749</v>
+        <v>0.06203</v>
       </c>
       <c r="E101" t="n">
-        <v>0.00458</v>
+        <v>0.01034</v>
       </c>
       <c r="F101" t="n">
-        <v>2.54116</v>
+        <v>2.90111</v>
       </c>
       <c r="G101" t="n">
         <v>0.85</v>
@@ -3083,16 +3083,16 @@
         <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D102" t="n">
-        <v>0.03779</v>
+        <v>0.08071</v>
       </c>
       <c r="E102" t="n">
-        <v>0.0063</v>
+        <v>0.01345</v>
       </c>
       <c r="F102" t="n">
-        <v>1.6576</v>
+        <v>3.46812</v>
       </c>
       <c r="G102" t="n">
         <v>0.15</v>
@@ -3109,16 +3109,16 @@
         <v>1</v>
       </c>
       <c r="C103" t="n">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="D103" t="n">
-        <v>0.09200999999999999</v>
+        <v>0.08019999999999999</v>
       </c>
       <c r="E103" t="n">
-        <v>0.01534</v>
+        <v>0.01337</v>
       </c>
       <c r="F103" t="n">
-        <v>3.52227</v>
+        <v>3.74465</v>
       </c>
       <c r="G103" t="n">
         <v>0.15</v>
@@ -3135,16 +3135,16 @@
         <v>1</v>
       </c>
       <c r="C104" t="n">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D104" t="n">
-        <v>0.0672</v>
+        <v>0.04771</v>
       </c>
       <c r="E104" t="n">
-        <v>0.0112</v>
+        <v>0.00795</v>
       </c>
       <c r="F104" t="n">
-        <v>2.72707</v>
+        <v>3.20173</v>
       </c>
       <c r="G104" t="n">
         <v>0.15</v>
@@ -3161,16 +3161,16 @@
         <v>1</v>
       </c>
       <c r="C105" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D105" t="n">
-        <v>0.08186</v>
+        <v>0.12165</v>
       </c>
       <c r="E105" t="n">
-        <v>0.01364</v>
+        <v>0.02027</v>
       </c>
       <c r="F105" t="n">
-        <v>3.69481</v>
+        <v>4.71745</v>
       </c>
       <c r="G105" t="n">
         <v>0.15</v>
@@ -3187,16 +3187,16 @@
         <v>1</v>
       </c>
       <c r="C106" t="n">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="D106" t="n">
-        <v>0.10074</v>
+        <v>0.10483</v>
       </c>
       <c r="E106" t="n">
-        <v>0.01679</v>
+        <v>0.01747</v>
       </c>
       <c r="F106" t="n">
-        <v>3.43807</v>
+        <v>5.10104</v>
       </c>
       <c r="G106" t="n">
         <v>0.15</v>
@@ -3213,16 +3213,16 @@
         <v>1</v>
       </c>
       <c r="C107" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D107" t="n">
-        <v>0.08187</v>
+        <v>0.08669</v>
       </c>
       <c r="E107" t="n">
-        <v>0.01365</v>
+        <v>0.01445</v>
       </c>
       <c r="F107" t="n">
-        <v>4.24106</v>
+        <v>3.80843</v>
       </c>
       <c r="G107" t="n">
         <v>0.15</v>
@@ -3239,16 +3239,16 @@
         <v>1</v>
       </c>
       <c r="C108" t="n">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D108" t="n">
-        <v>0.06875000000000001</v>
+        <v>0.04682</v>
       </c>
       <c r="E108" t="n">
-        <v>0.01146</v>
+        <v>0.0078</v>
       </c>
       <c r="F108" t="n">
-        <v>2.40085</v>
+        <v>2.33028</v>
       </c>
       <c r="G108" t="n">
         <v>0.15</v>
@@ -3265,16 +3265,16 @@
         <v>1</v>
       </c>
       <c r="C109" t="n">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D109" t="n">
-        <v>0.07063999999999999</v>
+        <v>0.05432</v>
       </c>
       <c r="E109" t="n">
-        <v>0.01177</v>
+        <v>0.009050000000000001</v>
       </c>
       <c r="F109" t="n">
-        <v>2.35194</v>
+        <v>2.13216</v>
       </c>
       <c r="G109" t="n">
         <v>0.15</v>
@@ -3291,16 +3291,16 @@
         <v>1</v>
       </c>
       <c r="C110" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D110" t="n">
-        <v>0.05807</v>
+        <v>0.04988</v>
       </c>
       <c r="E110" t="n">
-        <v>0.009679999999999999</v>
+        <v>0.00831</v>
       </c>
       <c r="F110" t="n">
-        <v>2.20118</v>
+        <v>1.74435</v>
       </c>
       <c r="G110" t="n">
         <v>0.15</v>
@@ -3317,16 +3317,16 @@
         <v>1</v>
       </c>
       <c r="C111" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D111" t="n">
-        <v>0.0757</v>
+        <v>0.10094</v>
       </c>
       <c r="E111" t="n">
-        <v>0.01262</v>
+        <v>0.01682</v>
       </c>
       <c r="F111" t="n">
-        <v>3.54579</v>
+        <v>5.14472</v>
       </c>
       <c r="G111" t="n">
         <v>0.15</v>
@@ -3343,16 +3343,16 @@
         <v>1</v>
       </c>
       <c r="C112" t="n">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D112" t="n">
-        <v>0.04374</v>
+        <v>0.15073</v>
       </c>
       <c r="E112" t="n">
-        <v>0.00729</v>
+        <v>0.02512</v>
       </c>
       <c r="F112" t="n">
-        <v>2.09151</v>
+        <v>3.85066</v>
       </c>
       <c r="G112" t="n">
         <v>0.15</v>
@@ -3369,16 +3369,16 @@
         <v>1</v>
       </c>
       <c r="C113" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D113" t="n">
-        <v>0.06802</v>
+        <v>0.11283</v>
       </c>
       <c r="E113" t="n">
-        <v>0.01134</v>
+        <v>0.01881</v>
       </c>
       <c r="F113" t="n">
-        <v>3.90683</v>
+        <v>5.82066</v>
       </c>
       <c r="G113" t="n">
         <v>0.15</v>
@@ -3395,16 +3395,16 @@
         <v>1</v>
       </c>
       <c r="C114" t="n">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="D114" t="n">
-        <v>0.16389</v>
+        <v>0.04198</v>
       </c>
       <c r="E114" t="n">
-        <v>0.02731</v>
+        <v>0.007</v>
       </c>
       <c r="F114" t="n">
-        <v>3.90716</v>
+        <v>2.61266</v>
       </c>
       <c r="G114" t="n">
         <v>0.15</v>
@@ -3421,16 +3421,16 @@
         <v>1</v>
       </c>
       <c r="C115" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D115" t="n">
-        <v>0.07413</v>
+        <v>0.02881</v>
       </c>
       <c r="E115" t="n">
-        <v>0.01235</v>
+        <v>0.0048</v>
       </c>
       <c r="F115" t="n">
-        <v>2.91377</v>
+        <v>1.61073</v>
       </c>
       <c r="G115" t="n">
         <v>0.15</v>
@@ -3447,16 +3447,16 @@
         <v>1</v>
       </c>
       <c r="C116" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D116" t="n">
-        <v>0.06216</v>
+        <v>0.05023</v>
       </c>
       <c r="E116" t="n">
-        <v>0.01036</v>
+        <v>0.008370000000000001</v>
       </c>
       <c r="F116" t="n">
-        <v>3.65326</v>
+        <v>3.37098</v>
       </c>
       <c r="G116" t="n">
         <v>0.15</v>
@@ -3473,16 +3473,16 @@
         <v>1</v>
       </c>
       <c r="C117" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D117" t="n">
-        <v>0.05779</v>
+        <v>0.08375</v>
       </c>
       <c r="E117" t="n">
-        <v>0.00963</v>
+        <v>0.01396</v>
       </c>
       <c r="F117" t="n">
-        <v>2.1598</v>
+        <v>3.58987</v>
       </c>
       <c r="G117" t="n">
         <v>0.15</v>
@@ -3499,16 +3499,16 @@
         <v>1</v>
       </c>
       <c r="C118" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D118" t="n">
-        <v>0.02838</v>
+        <v>0.07925</v>
       </c>
       <c r="E118" t="n">
-        <v>0.00473</v>
+        <v>0.01321</v>
       </c>
       <c r="F118" t="n">
-        <v>1.3653</v>
+        <v>3.59438</v>
       </c>
       <c r="G118" t="n">
         <v>0.15</v>
@@ -3525,16 +3525,16 @@
         <v>1</v>
       </c>
       <c r="C119" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D119" t="n">
-        <v>0.05763</v>
+        <v>0.03066</v>
       </c>
       <c r="E119" t="n">
-        <v>0.009599999999999999</v>
+        <v>0.00511</v>
       </c>
       <c r="F119" t="n">
-        <v>1.95811</v>
+        <v>1.76132</v>
       </c>
       <c r="G119" t="n">
         <v>0.15</v>
@@ -3551,16 +3551,16 @@
         <v>1</v>
       </c>
       <c r="C120" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D120" t="n">
-        <v>0.03923</v>
+        <v>0.0477</v>
       </c>
       <c r="E120" t="n">
-        <v>0.00654</v>
+        <v>0.00795</v>
       </c>
       <c r="F120" t="n">
-        <v>1.19968</v>
+        <v>1.58044</v>
       </c>
       <c r="G120" t="n">
         <v>0.15</v>
@@ -3577,16 +3577,16 @@
         <v>1</v>
       </c>
       <c r="C121" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="D121" t="n">
-        <v>0.04922</v>
+        <v>0.02552</v>
       </c>
       <c r="E121" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.00425</v>
       </c>
       <c r="F121" t="n">
-        <v>1.50295</v>
+        <v>1.42689</v>
       </c>
       <c r="G121" t="n">
         <v>0.15</v>
@@ -3603,16 +3603,16 @@
         <v>1</v>
       </c>
       <c r="C122" t="n">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D122" t="n">
-        <v>0.046</v>
+        <v>0.09037000000000001</v>
       </c>
       <c r="E122" t="n">
-        <v>0.00575</v>
+        <v>0.0113</v>
       </c>
       <c r="F122" t="n">
-        <v>1.24</v>
+        <v>3.42393</v>
       </c>
       <c r="G122" t="n">
         <v>0.15</v>
@@ -3629,16 +3629,16 @@
         <v>1</v>
       </c>
       <c r="C123" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D123" t="n">
-        <v>0.06327000000000001</v>
+        <v>0.08913</v>
       </c>
       <c r="E123" t="n">
-        <v>0.00791</v>
+        <v>0.01114</v>
       </c>
       <c r="F123" t="n">
-        <v>1.08158</v>
+        <v>2.14221</v>
       </c>
       <c r="G123" t="n">
         <v>0.15</v>
@@ -3655,16 +3655,16 @@
         <v>1</v>
       </c>
       <c r="C124" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D124" t="n">
-        <v>0.04646</v>
+        <v>0.08422</v>
       </c>
       <c r="E124" t="n">
-        <v>0.00581</v>
+        <v>0.01053</v>
       </c>
       <c r="F124" t="n">
-        <v>1.74684</v>
+        <v>2.13958</v>
       </c>
       <c r="G124" t="n">
         <v>0.15</v>
@@ -3681,16 +3681,16 @@
         <v>1</v>
       </c>
       <c r="C125" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D125" t="n">
-        <v>0.08196000000000001</v>
+        <v>0.09166000000000001</v>
       </c>
       <c r="E125" t="n">
-        <v>0.01024</v>
+        <v>0.01146</v>
       </c>
       <c r="F125" t="n">
-        <v>1.74334</v>
+        <v>2.47652</v>
       </c>
       <c r="G125" t="n">
         <v>0.15</v>
@@ -3710,13 +3710,13 @@
         <v>21</v>
       </c>
       <c r="D126" t="n">
-        <v>0.06994</v>
+        <v>0.08110000000000001</v>
       </c>
       <c r="E126" t="n">
-        <v>0.00874</v>
+        <v>0.01014</v>
       </c>
       <c r="F126" t="n">
-        <v>2.86576</v>
+        <v>3.00955</v>
       </c>
       <c r="G126" t="n">
         <v>0.15</v>
@@ -3733,16 +3733,16 @@
         <v>1</v>
       </c>
       <c r="C127" t="n">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D127" t="n">
-        <v>0.10689</v>
+        <v>0.07655000000000001</v>
       </c>
       <c r="E127" t="n">
-        <v>0.01336</v>
+        <v>0.00957</v>
       </c>
       <c r="F127" t="n">
-        <v>2.84897</v>
+        <v>3.36155</v>
       </c>
       <c r="G127" t="n">
         <v>0.15</v>
@@ -3759,16 +3759,16 @@
         <v>1</v>
       </c>
       <c r="C128" t="n">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D128" t="n">
-        <v>0.10427</v>
+        <v>0.10625</v>
       </c>
       <c r="E128" t="n">
-        <v>0.01303</v>
+        <v>0.01328</v>
       </c>
       <c r="F128" t="n">
-        <v>4.22688</v>
+        <v>2.95424</v>
       </c>
       <c r="G128" t="n">
         <v>0.15</v>
@@ -3785,16 +3785,16 @@
         <v>1</v>
       </c>
       <c r="C129" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D129" t="n">
-        <v>0.08452999999999999</v>
+        <v>0.17319</v>
       </c>
       <c r="E129" t="n">
-        <v>0.01057</v>
+        <v>0.02165</v>
       </c>
       <c r="F129" t="n">
-        <v>2.69843</v>
+        <v>6.12526</v>
       </c>
       <c r="G129" t="n">
         <v>0.15</v>
@@ -3811,16 +3811,16 @@
         <v>1</v>
       </c>
       <c r="C130" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D130" t="n">
-        <v>0.12599</v>
+        <v>0.08448</v>
       </c>
       <c r="E130" t="n">
-        <v>0.01575</v>
+        <v>0.01056</v>
       </c>
       <c r="F130" t="n">
-        <v>3.23978</v>
+        <v>2.51272</v>
       </c>
       <c r="G130" t="n">
         <v>0.15</v>
@@ -3837,16 +3837,16 @@
         <v>1</v>
       </c>
       <c r="C131" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D131" t="n">
-        <v>0.05908</v>
+        <v>0.10289</v>
       </c>
       <c r="E131" t="n">
-        <v>0.00738</v>
+        <v>0.01286</v>
       </c>
       <c r="F131" t="n">
-        <v>2.02339</v>
+        <v>2.28729</v>
       </c>
       <c r="G131" t="n">
         <v>0.15</v>
@@ -3863,16 +3863,16 @@
         <v>1</v>
       </c>
       <c r="C132" t="n">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D132" t="n">
-        <v>0.08649999999999999</v>
+        <v>0.06448</v>
       </c>
       <c r="E132" t="n">
-        <v>0.01081</v>
+        <v>0.008059999999999999</v>
       </c>
       <c r="F132" t="n">
-        <v>3.28848</v>
+        <v>2.97615</v>
       </c>
       <c r="G132" t="n">
         <v>0.15</v>
@@ -3889,16 +3889,16 @@
         <v>1</v>
       </c>
       <c r="C133" t="n">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D133" t="n">
-        <v>0.08996</v>
+        <v>0.07597</v>
       </c>
       <c r="E133" t="n">
-        <v>0.01124</v>
+        <v>0.0095</v>
       </c>
       <c r="F133" t="n">
-        <v>2.94856</v>
+        <v>3.48625</v>
       </c>
       <c r="G133" t="n">
         <v>0.15</v>
@@ -3915,16 +3915,16 @@
         <v>1</v>
       </c>
       <c r="C134" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D134" t="n">
-        <v>0.10209</v>
+        <v>0.06198</v>
       </c>
       <c r="E134" t="n">
-        <v>0.01276</v>
+        <v>0.00775</v>
       </c>
       <c r="F134" t="n">
-        <v>3.64762</v>
+        <v>3.01176</v>
       </c>
       <c r="G134" t="n">
         <v>0.15</v>
@@ -3941,16 +3941,16 @@
         <v>1</v>
       </c>
       <c r="C135" t="n">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D135" t="n">
-        <v>0.06564</v>
+        <v>0.14251</v>
       </c>
       <c r="E135" t="n">
-        <v>0.008200000000000001</v>
+        <v>0.01781</v>
       </c>
       <c r="F135" t="n">
-        <v>3.42771</v>
+        <v>3.37675</v>
       </c>
       <c r="G135" t="n">
         <v>0.15</v>
@@ -3967,16 +3967,16 @@
         <v>1</v>
       </c>
       <c r="C136" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D136" t="n">
-        <v>0.05768</v>
+        <v>0.05893</v>
       </c>
       <c r="E136" t="n">
-        <v>0.00721</v>
+        <v>0.00737</v>
       </c>
       <c r="F136" t="n">
-        <v>1.30615</v>
+        <v>2.53008</v>
       </c>
       <c r="G136" t="n">
         <v>0.15</v>
@@ -3993,16 +3993,16 @@
         <v>1</v>
       </c>
       <c r="C137" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D137" t="n">
-        <v>0.02898</v>
+        <v>0.1486</v>
       </c>
       <c r="E137" t="n">
-        <v>0.00362</v>
+        <v>0.01858</v>
       </c>
       <c r="F137" t="n">
-        <v>1.26269</v>
+        <v>4.43736</v>
       </c>
       <c r="G137" t="n">
         <v>0.15</v>
@@ -4019,16 +4019,16 @@
         <v>1</v>
       </c>
       <c r="C138" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D138" t="n">
-        <v>0.05305</v>
+        <v>0.04274</v>
       </c>
       <c r="E138" t="n">
-        <v>0.00663</v>
+        <v>0.00534</v>
       </c>
       <c r="F138" t="n">
-        <v>2.46158</v>
+        <v>1.45034</v>
       </c>
       <c r="G138" t="n">
         <v>0.15</v>
@@ -4045,16 +4045,16 @@
         <v>1</v>
       </c>
       <c r="C139" t="n">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="D139" t="n">
-        <v>0.03853</v>
+        <v>0.10469</v>
       </c>
       <c r="E139" t="n">
-        <v>0.00482</v>
+        <v>0.01309</v>
       </c>
       <c r="F139" t="n">
-        <v>2.13771</v>
+        <v>2.91587</v>
       </c>
       <c r="G139" t="n">
         <v>0.15</v>
@@ -4071,16 +4071,16 @@
         <v>1</v>
       </c>
       <c r="C140" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="D140" t="n">
-        <v>0.104</v>
+        <v>0.06367</v>
       </c>
       <c r="E140" t="n">
-        <v>0.013</v>
+        <v>0.00796</v>
       </c>
       <c r="F140" t="n">
-        <v>2.25356</v>
+        <v>3.69694</v>
       </c>
       <c r="G140" t="n">
         <v>0.15</v>
@@ -4097,16 +4097,16 @@
         <v>1</v>
       </c>
       <c r="C141" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D141" t="n">
-        <v>0.05851</v>
+        <v>0.09379999999999999</v>
       </c>
       <c r="E141" t="n">
-        <v>0.00731</v>
+        <v>0.01172</v>
       </c>
       <c r="F141" t="n">
-        <v>2.92302</v>
+        <v>3.27634</v>
       </c>
       <c r="G141" t="n">
         <v>0.15</v>
@@ -4123,16 +4123,16 @@
         <v>1</v>
       </c>
       <c r="C142" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D142" t="n">
-        <v>0.02799</v>
+        <v>0.06407</v>
       </c>
       <c r="E142" t="n">
-        <v>0.0035</v>
+        <v>0.00801</v>
       </c>
       <c r="F142" t="n">
-        <v>1.34925</v>
+        <v>2.30106</v>
       </c>
       <c r="G142" t="n">
         <v>0.85</v>
@@ -4149,16 +4149,16 @@
         <v>1</v>
       </c>
       <c r="C143" t="n">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D143" t="n">
-        <v>0.06167</v>
+        <v>0.0706</v>
       </c>
       <c r="E143" t="n">
-        <v>0.00771</v>
+        <v>0.00882</v>
       </c>
       <c r="F143" t="n">
-        <v>1.83696</v>
+        <v>3.22855</v>
       </c>
       <c r="G143" t="n">
         <v>0.85</v>
@@ -4175,16 +4175,16 @@
         <v>1</v>
       </c>
       <c r="C144" t="n">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D144" t="n">
-        <v>0.07523000000000001</v>
+        <v>0.05006</v>
       </c>
       <c r="E144" t="n">
-        <v>0.0094</v>
+        <v>0.00626</v>
       </c>
       <c r="F144" t="n">
-        <v>2.48001</v>
+        <v>2.12929</v>
       </c>
       <c r="G144" t="n">
         <v>0.85</v>
@@ -4201,16 +4201,16 @@
         <v>1</v>
       </c>
       <c r="C145" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D145" t="n">
-        <v>0.02124</v>
+        <v>0.03747</v>
       </c>
       <c r="E145" t="n">
-        <v>0.00265</v>
+        <v>0.00468</v>
       </c>
       <c r="F145" t="n">
-        <v>1.41529</v>
+        <v>1.50177</v>
       </c>
       <c r="G145" t="n">
         <v>0.85</v>
@@ -4227,16 +4227,16 @@
         <v>1</v>
       </c>
       <c r="C146" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D146" t="n">
-        <v>0.03272</v>
+        <v>0.01551</v>
       </c>
       <c r="E146" t="n">
-        <v>0.00409</v>
+        <v>0.00194</v>
       </c>
       <c r="F146" t="n">
-        <v>1.19748</v>
+        <v>1.04161</v>
       </c>
       <c r="G146" t="n">
         <v>0.85</v>
@@ -4256,13 +4256,13 @@
         <v>20</v>
       </c>
       <c r="D147" t="n">
-        <v>0.02472</v>
+        <v>0.02396</v>
       </c>
       <c r="E147" t="n">
-        <v>0.00309</v>
+        <v>0.003</v>
       </c>
       <c r="F147" t="n">
-        <v>1.04033</v>
+        <v>1.23119</v>
       </c>
       <c r="G147" t="n">
         <v>0.85</v>
@@ -4279,16 +4279,16 @@
         <v>1</v>
       </c>
       <c r="C148" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D148" t="n">
-        <v>0.10107</v>
+        <v>0.04121</v>
       </c>
       <c r="E148" t="n">
-        <v>0.01263</v>
+        <v>0.00515</v>
       </c>
       <c r="F148" t="n">
-        <v>2.41941</v>
+        <v>1.64694</v>
       </c>
       <c r="G148" t="n">
         <v>0.85</v>
@@ -4305,16 +4305,16 @@
         <v>1</v>
       </c>
       <c r="C149" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D149" t="n">
-        <v>0.03577</v>
+        <v>0.08999</v>
       </c>
       <c r="E149" t="n">
-        <v>0.00447</v>
+        <v>0.01125</v>
       </c>
       <c r="F149" t="n">
-        <v>1.60696</v>
+        <v>2.53894</v>
       </c>
       <c r="G149" t="n">
         <v>0.85</v>
@@ -4331,16 +4331,16 @@
         <v>1</v>
       </c>
       <c r="C150" t="n">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="D150" t="n">
-        <v>0.0442</v>
+        <v>0.06214</v>
       </c>
       <c r="E150" t="n">
-        <v>0.00553</v>
+        <v>0.00777</v>
       </c>
       <c r="F150" t="n">
-        <v>1.44296</v>
+        <v>2.87773</v>
       </c>
       <c r="G150" t="n">
         <v>0.85</v>
@@ -4357,16 +4357,16 @@
         <v>1</v>
       </c>
       <c r="C151" t="n">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D151" t="n">
-        <v>0.02573</v>
+        <v>0.0488</v>
       </c>
       <c r="E151" t="n">
-        <v>0.00322</v>
+        <v>0.0061</v>
       </c>
       <c r="F151" t="n">
-        <v>1.34061</v>
+        <v>2.33837</v>
       </c>
       <c r="G151" t="n">
         <v>0.85</v>
@@ -4383,16 +4383,16 @@
         <v>1</v>
       </c>
       <c r="C152" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D152" t="n">
-        <v>0.03509</v>
+        <v>0.01704</v>
       </c>
       <c r="E152" t="n">
-        <v>0.00439</v>
+        <v>0.00213</v>
       </c>
       <c r="F152" t="n">
-        <v>1.82487</v>
+        <v>1.06465</v>
       </c>
       <c r="G152" t="n">
         <v>0.85</v>
@@ -4409,16 +4409,16 @@
         <v>1</v>
       </c>
       <c r="C153" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D153" t="n">
-        <v>0.02239</v>
+        <v>0.03067</v>
       </c>
       <c r="E153" t="n">
-        <v>0.0028</v>
+        <v>0.00383</v>
       </c>
       <c r="F153" t="n">
-        <v>1.05395</v>
+        <v>1.32853</v>
       </c>
       <c r="G153" t="n">
         <v>0.85</v>
@@ -4435,16 +4435,16 @@
         <v>1</v>
       </c>
       <c r="C154" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D154" t="n">
-        <v>0.01891</v>
+        <v>0.0427</v>
       </c>
       <c r="E154" t="n">
-        <v>0.00236</v>
+        <v>0.00534</v>
       </c>
       <c r="F154" t="n">
-        <v>1.14827</v>
+        <v>1.10808</v>
       </c>
       <c r="G154" t="n">
         <v>0.85</v>
@@ -4461,16 +4461,16 @@
         <v>1</v>
       </c>
       <c r="C155" t="n">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="D155" t="n">
-        <v>0.03905</v>
+        <v>0.0505</v>
       </c>
       <c r="E155" t="n">
-        <v>0.00488</v>
+        <v>0.00631</v>
       </c>
       <c r="F155" t="n">
-        <v>2.20229</v>
+        <v>1.70144</v>
       </c>
       <c r="G155" t="n">
         <v>0.85</v>
@@ -4487,16 +4487,16 @@
         <v>1</v>
       </c>
       <c r="C156" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="D156" t="n">
-        <v>0.04566</v>
+        <v>0.03226</v>
       </c>
       <c r="E156" t="n">
-        <v>0.00571</v>
+        <v>0.00403</v>
       </c>
       <c r="F156" t="n">
-        <v>1.9389</v>
+        <v>1.62068</v>
       </c>
       <c r="G156" t="n">
         <v>0.85</v>
@@ -4513,16 +4513,16 @@
         <v>1</v>
       </c>
       <c r="C157" t="n">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="D157" t="n">
-        <v>0.04509</v>
+        <v>0.02591</v>
       </c>
       <c r="E157" t="n">
-        <v>0.00564</v>
+        <v>0.00324</v>
       </c>
       <c r="F157" t="n">
-        <v>1.9047</v>
+        <v>1.38327</v>
       </c>
       <c r="G157" t="n">
         <v>0.85</v>
@@ -4539,16 +4539,16 @@
         <v>1</v>
       </c>
       <c r="C158" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D158" t="n">
-        <v>0.0708</v>
+        <v>0.02412</v>
       </c>
       <c r="E158" t="n">
-        <v>0.00885</v>
+        <v>0.00301</v>
       </c>
       <c r="F158" t="n">
-        <v>2.64401</v>
+        <v>1.11434</v>
       </c>
       <c r="G158" t="n">
         <v>0.85</v>
@@ -4565,16 +4565,16 @@
         <v>1</v>
       </c>
       <c r="C159" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D159" t="n">
-        <v>0.05298</v>
+        <v>0.04681</v>
       </c>
       <c r="E159" t="n">
-        <v>0.00662</v>
+        <v>0.00585</v>
       </c>
       <c r="F159" t="n">
-        <v>2.09463</v>
+        <v>1.67888</v>
       </c>
       <c r="G159" t="n">
         <v>0.85</v>
@@ -4591,16 +4591,16 @@
         <v>1</v>
       </c>
       <c r="C160" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D160" t="n">
-        <v>0.04635</v>
+        <v>0.03385</v>
       </c>
       <c r="E160" t="n">
-        <v>0.00579</v>
+        <v>0.00423</v>
       </c>
       <c r="F160" t="n">
-        <v>2.03046</v>
+        <v>1.433</v>
       </c>
       <c r="G160" t="n">
         <v>0.85</v>
@@ -4617,16 +4617,16 @@
         <v>1</v>
       </c>
       <c r="C161" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D161" t="n">
-        <v>0.01004</v>
+        <v>0.0358</v>
       </c>
       <c r="E161" t="n">
-        <v>0.00126</v>
+        <v>0.00447</v>
       </c>
       <c r="F161" t="n">
-        <v>0.89089</v>
+        <v>1.25975</v>
       </c>
       <c r="G161" t="n">
         <v>0.85</v>
@@ -4646,13 +4646,13 @@
         <v>10</v>
       </c>
       <c r="D162" t="n">
-        <v>0.009209999999999999</v>
+        <v>0.05972</v>
       </c>
       <c r="E162" t="n">
-        <v>0.00092</v>
+        <v>0.00597</v>
       </c>
       <c r="F162" t="n">
-        <v>0.64142</v>
+        <v>1.32981</v>
       </c>
       <c r="G162" t="n">
         <v>0.85</v>
@@ -4669,16 +4669,16 @@
         <v>1</v>
       </c>
       <c r="C163" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D163" t="n">
-        <v>0.05339</v>
+        <v>0.01347</v>
       </c>
       <c r="E163" t="n">
-        <v>0.00534</v>
+        <v>0.00135</v>
       </c>
       <c r="F163" t="n">
-        <v>1.18604</v>
+        <v>0.96658</v>
       </c>
       <c r="G163" t="n">
         <v>0.85</v>
@@ -4695,16 +4695,16 @@
         <v>1</v>
       </c>
       <c r="C164" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D164" t="n">
-        <v>0.05462</v>
+        <v>0.04116</v>
       </c>
       <c r="E164" t="n">
-        <v>0.00546</v>
+        <v>0.00412</v>
       </c>
       <c r="F164" t="n">
-        <v>2.25257</v>
+        <v>0.98197</v>
       </c>
       <c r="G164" t="n">
         <v>0.85</v>
@@ -4721,16 +4721,16 @@
         <v>1</v>
       </c>
       <c r="C165" t="n">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="D165" t="n">
-        <v>0.0806</v>
+        <v>0.03593</v>
       </c>
       <c r="E165" t="n">
-        <v>0.008059999999999999</v>
+        <v>0.00359</v>
       </c>
       <c r="F165" t="n">
-        <v>1.76469</v>
+        <v>1.34079</v>
       </c>
       <c r="G165" t="n">
         <v>0.85</v>
@@ -4747,16 +4747,16 @@
         <v>1</v>
       </c>
       <c r="C166" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D166" t="n">
-        <v>0.02238</v>
+        <v>0.02692</v>
       </c>
       <c r="E166" t="n">
-        <v>0.00224</v>
+        <v>0.00269</v>
       </c>
       <c r="F166" t="n">
-        <v>0.90783</v>
+        <v>0.90203</v>
       </c>
       <c r="G166" t="n">
         <v>0.85</v>
@@ -4773,16 +4773,16 @@
         <v>1</v>
       </c>
       <c r="C167" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D167" t="n">
-        <v>0.05248</v>
+        <v>0.02602</v>
       </c>
       <c r="E167" t="n">
-        <v>0.00525</v>
+        <v>0.0026</v>
       </c>
       <c r="F167" t="n">
-        <v>1.1403</v>
+        <v>0.86956</v>
       </c>
       <c r="G167" t="n">
         <v>0.85</v>
@@ -4802,13 +4802,13 @@
         <v>16</v>
       </c>
       <c r="D168" t="n">
-        <v>0.03953</v>
+        <v>0.06614</v>
       </c>
       <c r="E168" t="n">
-        <v>0.00395</v>
+        <v>0.00661</v>
       </c>
       <c r="F168" t="n">
-        <v>1.22048</v>
+        <v>1.70354</v>
       </c>
       <c r="G168" t="n">
         <v>0.85</v>
@@ -4825,16 +4825,16 @@
         <v>1</v>
       </c>
       <c r="C169" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D169" t="n">
-        <v>0.04103</v>
+        <v>0.0278</v>
       </c>
       <c r="E169" t="n">
-        <v>0.0041</v>
+        <v>0.00278</v>
       </c>
       <c r="F169" t="n">
-        <v>1.56466</v>
+        <v>0.82338</v>
       </c>
       <c r="G169" t="n">
         <v>0.85</v>
@@ -4851,16 +4851,16 @@
         <v>1</v>
       </c>
       <c r="C170" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D170" t="n">
-        <v>0.04104</v>
+        <v>0.02529</v>
       </c>
       <c r="E170" t="n">
-        <v>0.0041</v>
+        <v>0.00253</v>
       </c>
       <c r="F170" t="n">
-        <v>1.56645</v>
+        <v>1.20593</v>
       </c>
       <c r="G170" t="n">
         <v>0.85</v>
@@ -4877,16 +4877,16 @@
         <v>1</v>
       </c>
       <c r="C171" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D171" t="n">
-        <v>0.03464</v>
+        <v>0.02908</v>
       </c>
       <c r="E171" t="n">
-        <v>0.00346</v>
+        <v>0.00291</v>
       </c>
       <c r="F171" t="n">
-        <v>1.14845</v>
+        <v>0.86094</v>
       </c>
       <c r="G171" t="n">
         <v>0.85</v>
@@ -4903,16 +4903,16 @@
         <v>1</v>
       </c>
       <c r="C172" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D172" t="n">
-        <v>0.02484</v>
+        <v>0.0437</v>
       </c>
       <c r="E172" t="n">
-        <v>0.00248</v>
+        <v>0.00437</v>
       </c>
       <c r="F172" t="n">
-        <v>0.9186800000000001</v>
+        <v>1.22669</v>
       </c>
       <c r="G172" t="n">
         <v>0.85</v>
@@ -4929,16 +4929,16 @@
         <v>1</v>
       </c>
       <c r="C173" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D173" t="n">
-        <v>0.04518</v>
+        <v>0.07502</v>
       </c>
       <c r="E173" t="n">
-        <v>0.00452</v>
+        <v>0.0075</v>
       </c>
       <c r="F173" t="n">
-        <v>1.55847</v>
+        <v>2.15837</v>
       </c>
       <c r="G173" t="n">
         <v>0.85</v>
@@ -4955,16 +4955,16 @@
         <v>1</v>
       </c>
       <c r="C174" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D174" t="n">
-        <v>0.08588999999999999</v>
+        <v>0.04677</v>
       </c>
       <c r="E174" t="n">
-        <v>0.00859</v>
+        <v>0.00468</v>
       </c>
       <c r="F174" t="n">
-        <v>2.33643</v>
+        <v>1.84383</v>
       </c>
       <c r="G174" t="n">
         <v>0.85</v>
@@ -4981,16 +4981,16 @@
         <v>1</v>
       </c>
       <c r="C175" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D175" t="n">
-        <v>0.01941</v>
+        <v>0.05091</v>
       </c>
       <c r="E175" t="n">
-        <v>0.00194</v>
+        <v>0.00509</v>
       </c>
       <c r="F175" t="n">
-        <v>0.86053</v>
+        <v>1.53043</v>
       </c>
       <c r="G175" t="n">
         <v>0.85</v>
@@ -5007,16 +5007,16 @@
         <v>1</v>
       </c>
       <c r="C176" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D176" t="n">
-        <v>0.03975</v>
+        <v>0.0336</v>
       </c>
       <c r="E176" t="n">
-        <v>0.00398</v>
+        <v>0.00336</v>
       </c>
       <c r="F176" t="n">
-        <v>0.971</v>
+        <v>1.40304</v>
       </c>
       <c r="G176" t="n">
         <v>0.85</v>
@@ -5033,16 +5033,16 @@
         <v>1</v>
       </c>
       <c r="C177" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D177" t="n">
-        <v>0.04446</v>
+        <v>0.01648</v>
       </c>
       <c r="E177" t="n">
-        <v>0.00445</v>
+        <v>0.00165</v>
       </c>
       <c r="F177" t="n">
-        <v>1.83965</v>
+        <v>0.6941000000000001</v>
       </c>
       <c r="G177" t="n">
         <v>0.85</v>
@@ -5059,16 +5059,16 @@
         <v>1</v>
       </c>
       <c r="C178" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D178" t="n">
-        <v>0.07799</v>
+        <v>0.035</v>
       </c>
       <c r="E178" t="n">
-        <v>0.0078</v>
+        <v>0.0035</v>
       </c>
       <c r="F178" t="n">
-        <v>1.86438</v>
+        <v>1.17744</v>
       </c>
       <c r="G178" t="n">
         <v>0.85</v>
@@ -5085,16 +5085,16 @@
         <v>1</v>
       </c>
       <c r="C179" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D179" t="n">
-        <v>0.04151</v>
+        <v>0.04759</v>
       </c>
       <c r="E179" t="n">
-        <v>0.00415</v>
+        <v>0.00476</v>
       </c>
       <c r="F179" t="n">
-        <v>1.6003</v>
+        <v>1.40141</v>
       </c>
       <c r="G179" t="n">
         <v>0.85</v>
@@ -5111,16 +5111,16 @@
         <v>1</v>
       </c>
       <c r="C180" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D180" t="n">
-        <v>0.05295</v>
+        <v>0.04455</v>
       </c>
       <c r="E180" t="n">
-        <v>0.0053</v>
+        <v>0.00446</v>
       </c>
       <c r="F180" t="n">
-        <v>1.84459</v>
+        <v>1.13288</v>
       </c>
       <c r="G180" t="n">
         <v>0.85</v>
@@ -5137,16 +5137,16 @@
         <v>1</v>
       </c>
       <c r="C181" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D181" t="n">
-        <v>0.06854</v>
+        <v>0.02141</v>
       </c>
       <c r="E181" t="n">
-        <v>0.00685</v>
+        <v>0.00214</v>
       </c>
       <c r="F181" t="n">
-        <v>2.25212</v>
+        <v>1.19329</v>
       </c>
       <c r="G181" t="n">
         <v>0.85</v>
@@ -5163,16 +5163,16 @@
         <v>1</v>
       </c>
       <c r="C182" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D182" t="n">
-        <v>0.23358</v>
+        <v>0.09761</v>
       </c>
       <c r="E182" t="n">
-        <v>0.02336</v>
+        <v>0.00976</v>
       </c>
       <c r="F182" t="n">
-        <v>5.92021</v>
+        <v>2.74472</v>
       </c>
       <c r="G182" t="n">
         <v>0.15</v>
@@ -5189,16 +5189,16 @@
         <v>1</v>
       </c>
       <c r="C183" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D183" t="n">
-        <v>0.07582</v>
+        <v>0.09746</v>
       </c>
       <c r="E183" t="n">
-        <v>0.00758</v>
+        <v>0.00975</v>
       </c>
       <c r="F183" t="n">
-        <v>1.6275</v>
+        <v>1.93633</v>
       </c>
       <c r="G183" t="n">
         <v>0.15</v>
@@ -5215,16 +5215,16 @@
         <v>1</v>
       </c>
       <c r="C184" t="n">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D184" t="n">
-        <v>0.05445</v>
+        <v>0.07171</v>
       </c>
       <c r="E184" t="n">
-        <v>0.00544</v>
+        <v>0.00717</v>
       </c>
       <c r="F184" t="n">
-        <v>2.55923</v>
+        <v>1.73779</v>
       </c>
       <c r="G184" t="n">
         <v>0.15</v>
@@ -5244,13 +5244,13 @@
         <v>22</v>
       </c>
       <c r="D185" t="n">
-        <v>0.03927</v>
+        <v>0.06970999999999999</v>
       </c>
       <c r="E185" t="n">
-        <v>0.00393</v>
+        <v>0.00697</v>
       </c>
       <c r="F185" t="n">
-        <v>1.66808</v>
+        <v>2.33462</v>
       </c>
       <c r="G185" t="n">
         <v>0.15</v>
@@ -5267,16 +5267,16 @@
         <v>1</v>
       </c>
       <c r="C186" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D186" t="n">
-        <v>0.05507</v>
+        <v>0.13462</v>
       </c>
       <c r="E186" t="n">
-        <v>0.00551</v>
+        <v>0.01346</v>
       </c>
       <c r="F186" t="n">
-        <v>1.48142</v>
+        <v>2.35099</v>
       </c>
       <c r="G186" t="n">
         <v>0.15</v>
@@ -5293,16 +5293,16 @@
         <v>1</v>
       </c>
       <c r="C187" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D187" t="n">
-        <v>0.06269</v>
+        <v>0.16605</v>
       </c>
       <c r="E187" t="n">
-        <v>0.00627</v>
+        <v>0.01661</v>
       </c>
       <c r="F187" t="n">
-        <v>1.89088</v>
+        <v>4.00267</v>
       </c>
       <c r="G187" t="n">
         <v>0.15</v>
@@ -5319,16 +5319,16 @@
         <v>1</v>
       </c>
       <c r="C188" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D188" t="n">
-        <v>0.08932</v>
+        <v>0.07479</v>
       </c>
       <c r="E188" t="n">
-        <v>0.00893</v>
+        <v>0.00748</v>
       </c>
       <c r="F188" t="n">
-        <v>1.65467</v>
+        <v>3.40595</v>
       </c>
       <c r="G188" t="n">
         <v>0.15</v>
@@ -5348,13 +5348,13 @@
         <v>13</v>
       </c>
       <c r="D189" t="n">
-        <v>0.04834</v>
+        <v>0.06383</v>
       </c>
       <c r="E189" t="n">
-        <v>0.00483</v>
+        <v>0.00638</v>
       </c>
       <c r="F189" t="n">
-        <v>1.55169</v>
+        <v>1.84837</v>
       </c>
       <c r="G189" t="n">
         <v>0.15</v>
@@ -5371,16 +5371,16 @@
         <v>1</v>
       </c>
       <c r="C190" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D190" t="n">
-        <v>0.09439</v>
+        <v>0.07833</v>
       </c>
       <c r="E190" t="n">
-        <v>0.00944</v>
+        <v>0.00783</v>
       </c>
       <c r="F190" t="n">
-        <v>1.27976</v>
+        <v>2.41957</v>
       </c>
       <c r="G190" t="n">
         <v>0.15</v>
@@ -5397,16 +5397,16 @@
         <v>1</v>
       </c>
       <c r="C191" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D191" t="n">
-        <v>0.0475</v>
+        <v>0.20628</v>
       </c>
       <c r="E191" t="n">
-        <v>0.00475</v>
+        <v>0.02063</v>
       </c>
       <c r="F191" t="n">
-        <v>1.53524</v>
+        <v>3.54755</v>
       </c>
       <c r="G191" t="n">
         <v>0.15</v>
@@ -5423,16 +5423,16 @@
         <v>1</v>
       </c>
       <c r="C192" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D192" t="n">
-        <v>0.11456</v>
+        <v>0.04369</v>
       </c>
       <c r="E192" t="n">
-        <v>0.01146</v>
+        <v>0.00437</v>
       </c>
       <c r="F192" t="n">
-        <v>3.72102</v>
+        <v>1.69838</v>
       </c>
       <c r="G192" t="n">
         <v>0.15</v>
@@ -5449,16 +5449,16 @@
         <v>1</v>
       </c>
       <c r="C193" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D193" t="n">
-        <v>0.10331</v>
+        <v>0.20746</v>
       </c>
       <c r="E193" t="n">
-        <v>0.01033</v>
+        <v>0.02075</v>
       </c>
       <c r="F193" t="n">
-        <v>4.10734</v>
+        <v>5.53032</v>
       </c>
       <c r="G193" t="n">
         <v>0.15</v>
@@ -5478,13 +5478,13 @@
         <v>12</v>
       </c>
       <c r="D194" t="n">
-        <v>0.1565</v>
+        <v>0.05827</v>
       </c>
       <c r="E194" t="n">
-        <v>0.01565</v>
+        <v>0.00583</v>
       </c>
       <c r="F194" t="n">
-        <v>3.35434</v>
+        <v>1.87232</v>
       </c>
       <c r="G194" t="n">
         <v>0.15</v>
@@ -5501,16 +5501,16 @@
         <v>1</v>
       </c>
       <c r="C195" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D195" t="n">
-        <v>0.1814</v>
+        <v>0.20158</v>
       </c>
       <c r="E195" t="n">
-        <v>0.01814</v>
+        <v>0.02016</v>
       </c>
       <c r="F195" t="n">
-        <v>3.74468</v>
+        <v>3.49274</v>
       </c>
       <c r="G195" t="n">
         <v>0.15</v>
@@ -5527,16 +5527,16 @@
         <v>1</v>
       </c>
       <c r="C196" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D196" t="n">
-        <v>0.11209</v>
+        <v>0.15667</v>
       </c>
       <c r="E196" t="n">
-        <v>0.01121</v>
+        <v>0.01567</v>
       </c>
       <c r="F196" t="n">
-        <v>3.12175</v>
+        <v>4.39914</v>
       </c>
       <c r="G196" t="n">
         <v>0.15</v>
@@ -5553,16 +5553,16 @@
         <v>1</v>
       </c>
       <c r="C197" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D197" t="n">
-        <v>0.02817</v>
+        <v>0.13164</v>
       </c>
       <c r="E197" t="n">
-        <v>0.00282</v>
+        <v>0.01316</v>
       </c>
       <c r="F197" t="n">
-        <v>1.34421</v>
+        <v>4.47036</v>
       </c>
       <c r="G197" t="n">
         <v>0.15</v>
@@ -5579,16 +5579,16 @@
         <v>1</v>
       </c>
       <c r="C198" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D198" t="n">
-        <v>0.0497</v>
+        <v>0.1206</v>
       </c>
       <c r="E198" t="n">
-        <v>0.00497</v>
+        <v>0.01206</v>
       </c>
       <c r="F198" t="n">
-        <v>1.71827</v>
+        <v>3.23454</v>
       </c>
       <c r="G198" t="n">
         <v>0.15</v>
@@ -5605,16 +5605,16 @@
         <v>1</v>
       </c>
       <c r="C199" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D199" t="n">
-        <v>0.14471</v>
+        <v>0.10898</v>
       </c>
       <c r="E199" t="n">
-        <v>0.01447</v>
+        <v>0.0109</v>
       </c>
       <c r="F199" t="n">
-        <v>3.56628</v>
+        <v>1.54459</v>
       </c>
       <c r="G199" t="n">
         <v>0.15</v>
@@ -5631,16 +5631,16 @@
         <v>1</v>
       </c>
       <c r="C200" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D200" t="n">
-        <v>0.15371</v>
+        <v>0.04919</v>
       </c>
       <c r="E200" t="n">
-        <v>0.01537</v>
+        <v>0.00492</v>
       </c>
       <c r="F200" t="n">
-        <v>3.15064</v>
+        <v>1.67109</v>
       </c>
       <c r="G200" t="n">
         <v>0.15</v>
@@ -5657,16 +5657,16 @@
         <v>1</v>
       </c>
       <c r="C201" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D201" t="n">
-        <v>0.18163</v>
+        <v>0.07142</v>
       </c>
       <c r="E201" t="n">
-        <v>0.01816</v>
+        <v>0.00714</v>
       </c>
       <c r="F201" t="n">
-        <v>4.1779</v>
+        <v>1.80216</v>
       </c>
       <c r="G201" t="n">
         <v>0.15</v>

</xml_diff>